<commit_message>
fixed bug for read in of # in excel file
</commit_message>
<xml_diff>
--- a/public/Labware Excel Input.xlsx
+++ b/public/Labware Excel Input.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="wKvA2Y0N+qJv8fAkGha3TGvyRIxApfrAJ5pjGarnPtM="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="EIfhzpWIdlmbtGuC++vMaOkDDmzHovN3EEMQTraMo+s="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="105">
   <si>
     <t>A hash in this column will prevent the row being read in</t>
   </si>
@@ -93,175 +93,178 @@
     <t>Boolean (TRUE/FALSE) indicating if the plate has an optically clear bottom (e.g., for imaging)</t>
   </si>
   <si>
+    <t>Hash</t>
+  </si>
+  <si>
+    <t>plate_name</t>
+  </si>
+  <si>
+    <t>manufacturer</t>
+  </si>
+  <si>
+    <t>catalog_number</t>
+  </si>
+  <si>
+    <t>num_rows</t>
+  </si>
+  <si>
+    <t>num_columns</t>
+  </si>
+  <si>
+    <t>plate_length_mm</t>
+  </si>
+  <si>
+    <t>plate_width_mm</t>
+  </si>
+  <si>
+    <t>plate_height_mm</t>
+  </si>
+  <si>
+    <t>plate_rigidity_scale</t>
+  </si>
+  <si>
+    <t>well_max_depth_mm</t>
+  </si>
+  <si>
+    <t>well_shape</t>
+  </si>
+  <si>
+    <t>well_bottom_shape</t>
+  </si>
+  <si>
+    <t>bottom_start_depth_mm</t>
+  </si>
+  <si>
+    <t>well_length_mm</t>
+  </si>
+  <si>
+    <t>well_width_mm</t>
+  </si>
+  <si>
+    <t>offset_left_to_a1_mm</t>
+  </si>
+  <si>
+    <t>offset_top_to_a1_mm</t>
+  </si>
+  <si>
+    <t>offset_right_to_final_well_mm</t>
+  </si>
+  <si>
+    <t>offset_bottom_to_final_well_mm</t>
+  </si>
+  <si>
+    <t>max_volume_ul</t>
+  </si>
+  <si>
+    <t>dead_volume_ul</t>
+  </si>
+  <si>
+    <t>surface_treatment</t>
+  </si>
+  <si>
+    <t>black_bottom</t>
+  </si>
+  <si>
+    <t>optical_bottom</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>96-well flat-bottom Corning clear</t>
+  </si>
+  <si>
+    <t>Corning</t>
+  </si>
+  <si>
+    <t>3013</t>
+  </si>
+  <si>
+    <t>circular</t>
+  </si>
+  <si>
+    <t>U-Bottom</t>
+  </si>
+  <si>
+    <t>TC-treated</t>
+  </si>
+  <si>
+    <t>This is a test plate</t>
+  </si>
+  <si>
+    <t>384-well V-bottom Greiner black</t>
+  </si>
+  <si>
+    <t>Greiner</t>
+  </si>
+  <si>
+    <t>3451</t>
+  </si>
+  <si>
+    <t>V-Bottom</t>
+  </si>
+  <si>
+    <t>untreated</t>
+  </si>
+  <si>
+    <t>96-well U-bottom ThermoFisher clear</t>
+  </si>
+  <si>
+    <t>ThermoFisher</t>
+  </si>
+  <si>
+    <t>3244</t>
+  </si>
+  <si>
+    <t>square</t>
+  </si>
+  <si>
+    <t>non-binding</t>
+  </si>
+  <si>
+    <t>1536-well V-bottom ThermoFisher clear</t>
+  </si>
+  <si>
+    <t>3173</t>
+  </si>
+  <si>
+    <t>384-well U-bottom Corning clear</t>
+  </si>
+  <si>
+    <t>3243</t>
+  </si>
+  <si>
+    <t>96-well V-bottom Nunc white</t>
+  </si>
+  <si>
+    <t>Nunc</t>
+  </si>
+  <si>
+    <t>3537</t>
+  </si>
+  <si>
+    <t>384-well U-bottom Greiner black</t>
+  </si>
+  <si>
+    <t>3730</t>
+  </si>
+  <si>
+    <t>384-well flat-bottom Corning black</t>
+  </si>
+  <si>
+    <t>3811</t>
+  </si>
+  <si>
+    <t>Flat</t>
+  </si>
+  <si>
+    <t>384-well V-bottom Corning white</t>
+  </si>
+  <si>
+    <t>3358</t>
+  </si>
+  <si>
     <t>#</t>
-  </si>
-  <si>
-    <t>plate_name</t>
-  </si>
-  <si>
-    <t>manufacturer</t>
-  </si>
-  <si>
-    <t>catalog_number</t>
-  </si>
-  <si>
-    <t>num_rows</t>
-  </si>
-  <si>
-    <t>num_columns</t>
-  </si>
-  <si>
-    <t>plate_length_mm</t>
-  </si>
-  <si>
-    <t>plate_width_mm</t>
-  </si>
-  <si>
-    <t>plate_height_mm</t>
-  </si>
-  <si>
-    <t>plate_rigidity_scale</t>
-  </si>
-  <si>
-    <t>well_max_depth_mm</t>
-  </si>
-  <si>
-    <t>well_shape</t>
-  </si>
-  <si>
-    <t>well_bottom_shape</t>
-  </si>
-  <si>
-    <t>bottom_start_depth_mm</t>
-  </si>
-  <si>
-    <t>well_length_mm</t>
-  </si>
-  <si>
-    <t>well_width_mm</t>
-  </si>
-  <si>
-    <t>offset_left_to_a1_mm</t>
-  </si>
-  <si>
-    <t>offset_top_to_a1_mm</t>
-  </si>
-  <si>
-    <t>offset_right_to_final_well_mm</t>
-  </si>
-  <si>
-    <t>offset_bottom_to_final_well_mm</t>
-  </si>
-  <si>
-    <t>max_volume_ul</t>
-  </si>
-  <si>
-    <t>dead_volume_ul</t>
-  </si>
-  <si>
-    <t>surface_treatment</t>
-  </si>
-  <si>
-    <t>black_bottom</t>
-  </si>
-  <si>
-    <t>optical_bottom</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>96-well flat-bottom Corning clear</t>
-  </si>
-  <si>
-    <t>Corning</t>
-  </si>
-  <si>
-    <t>3013</t>
-  </si>
-  <si>
-    <t>circular</t>
-  </si>
-  <si>
-    <t>U-Bottom</t>
-  </si>
-  <si>
-    <t>TC-treated</t>
-  </si>
-  <si>
-    <t>This is a test plate</t>
-  </si>
-  <si>
-    <t>384-well V-bottom Greiner black</t>
-  </si>
-  <si>
-    <t>Greiner</t>
-  </si>
-  <si>
-    <t>3451</t>
-  </si>
-  <si>
-    <t>V-Bottom</t>
-  </si>
-  <si>
-    <t>untreated</t>
-  </si>
-  <si>
-    <t>96-well U-bottom ThermoFisher clear</t>
-  </si>
-  <si>
-    <t>ThermoFisher</t>
-  </si>
-  <si>
-    <t>3244</t>
-  </si>
-  <si>
-    <t>square</t>
-  </si>
-  <si>
-    <t>non-binding</t>
-  </si>
-  <si>
-    <t>1536-well V-bottom ThermoFisher clear</t>
-  </si>
-  <si>
-    <t>3173</t>
-  </si>
-  <si>
-    <t>384-well U-bottom Corning clear</t>
-  </si>
-  <si>
-    <t>3243</t>
-  </si>
-  <si>
-    <t>96-well V-bottom Nunc white</t>
-  </si>
-  <si>
-    <t>Nunc</t>
-  </si>
-  <si>
-    <t>3537</t>
-  </si>
-  <si>
-    <t>384-well U-bottom Greiner black</t>
-  </si>
-  <si>
-    <t>3730</t>
-  </si>
-  <si>
-    <t>384-well flat-bottom Corning black</t>
-  </si>
-  <si>
-    <t>3811</t>
-  </si>
-  <si>
-    <t>Flat</t>
-  </si>
-  <si>
-    <t>384-well V-bottom Corning white</t>
-  </si>
-  <si>
-    <t>3358</t>
   </si>
   <si>
     <t>384-well V-bottom ThermoFisher black</t>
@@ -375,10 +378,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -618,7 +621,9 @@
     <col customWidth="1" min="16" max="16" width="14.86"/>
     <col customWidth="1" min="17" max="17" width="18.86"/>
     <col customWidth="1" min="18" max="18" width="21.29"/>
-    <col customWidth="1" min="19" max="22" width="14.43"/>
+    <col customWidth="1" min="19" max="20" width="14.43"/>
+    <col customWidth="1" min="21" max="21" width="16.29"/>
+    <col customWidth="1" min="22" max="22" width="17.14"/>
     <col customWidth="1" min="23" max="23" width="12.14"/>
     <col customWidth="1" min="24" max="24" width="14.86"/>
     <col customWidth="1" min="25" max="25" width="13.57"/>
@@ -706,79 +711,79 @@
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1477,16 +1482,16 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E12" s="1">
         <v>16.0</v>
@@ -1557,16 +1562,16 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E13" s="1">
         <v>32.0</v>
@@ -1637,13 +1642,13 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="B14" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E14" s="1">
         <v>16.0</v>
@@ -1714,13 +1719,13 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="B15" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E15" s="1">
         <v>32.0</v>
@@ -1791,13 +1796,13 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="B16" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E16" s="1">
         <v>16.0</v>
@@ -1868,13 +1873,13 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="B17" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E17" s="1">
         <v>16.0</v>
@@ -1945,13 +1950,13 @@
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="B18" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E18" s="1">
         <v>32.0</v>
@@ -2022,13 +2027,13 @@
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="B19" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E19" s="1">
         <v>8.0</v>
@@ -2099,13 +2104,13 @@
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="B20" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E20" s="1">
         <v>32.0</v>
@@ -2176,13 +2181,13 @@
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="B21" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E21" s="1">
         <v>8.0</v>
@@ -2253,13 +2258,13 @@
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="B22" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E22" s="1">
         <v>32.0</v>

</xml_diff>